<commit_message>
Pflichtenheft fertig v0.1 Process File New Use case Systemarchitektur PAP
</commit_message>
<xml_diff>
--- a/1. Analyse/Arbeitspakete.xlsx
+++ b/1. Analyse/Arbeitspakete.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>Phasen</t>
   </si>
@@ -82,16 +82,25 @@
     <t>WA-Kostenplan</t>
   </si>
   <si>
+    <t>Need Pricelist</t>
+  </si>
+  <si>
     <t>WA-Nutzwertanalyse</t>
   </si>
   <si>
+    <t>Need Gewichtung</t>
+  </si>
+  <si>
     <t>WA-Machbarkeitsstudie</t>
   </si>
   <si>
+    <t>Setzt Nutzwertanalyse vorraus</t>
+  </si>
+  <si>
     <t>Fragenkatalog</t>
   </si>
   <si>
-    <t>Sammeln der ergebenen Fragen, während der Analysen Phase</t>
+    <t>Sammeln der ergebenen Fragen, während der Analysen Phase, Besprechung mit Vorgesetzten &amp; Nadja</t>
   </si>
   <si>
     <t>Pflichtenheft</t>
@@ -125,12 +134,6 @@
   </si>
   <si>
     <t>System-Architektur</t>
-  </si>
-  <si>
-    <t>Stakeholderanalyse</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Testfallkatalog</t>
@@ -204,7 +207,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -235,13 +238,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -336,7 +332,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -411,10 +407,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -534,25 +526,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="49.4081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="49.4081632653061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="48.8673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="31.5765306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="48.8673469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,7 +585,7 @@
       </c>
       <c r="C2" s="5" t="n">
         <f aca="false">SUM(F2:F12)</f>
-        <v>2.25</v>
+        <v>10.75</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>9</v>
@@ -719,9 +711,13 @@
       <c r="E8" s="10" t="n">
         <v>0.25</v>
       </c>
-      <c r="F8" s="10"/>
+      <c r="F8" s="10" t="n">
+        <v>0.25</v>
+      </c>
       <c r="G8" s="9"/>
-      <c r="H8" s="11"/>
+      <c r="H8" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="L8" s="0"/>
       <c r="M8" s="0"/>
     </row>
@@ -730,14 +726,18 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E9" s="10" t="n">
         <v>0.25</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="F9" s="10" t="n">
+        <v>0.5</v>
+      </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="11"/>
+      <c r="H9" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="L9" s="0"/>
       <c r="M9" s="0"/>
     </row>
@@ -746,28 +746,32 @@
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E10" s="10" t="n">
         <v>0.5</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="11"/>
-    </row>
-    <row r="11" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E11" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F11" s="10"/>
+      <c r="F11" s="10" t="n">
+        <v>0.75</v>
+      </c>
       <c r="G11" s="12" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H11" s="11"/>
     </row>
@@ -776,20 +780,22 @@
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E12" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="F12" s="15"/>
+      <c r="F12" s="15" t="n">
+        <v>7</v>
+      </c>
       <c r="G12" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
@@ -801,23 +807,25 @@
     </row>
     <row r="14" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B14" s="5" t="n">
-        <f aca="false">SUM(E14:E23)</f>
+        <f aca="false">SUM(E14:E22)</f>
         <v>15</v>
       </c>
       <c r="C14" s="5" t="n">
-        <f aca="false">SUM(F14:F23)</f>
-        <v>0</v>
+        <f aca="false">SUM(F14:F22)</f>
+        <v>0.25</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E14" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7" t="n">
+        <v>0.25</v>
+      </c>
       <c r="G14" s="9"/>
       <c r="H14" s="11"/>
     </row>
@@ -826,7 +834,7 @@
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E15" s="10" t="n">
         <v>1</v>
@@ -840,7 +848,7 @@
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E16" s="10" t="n">
         <v>3</v>
@@ -854,7 +862,7 @@
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E17" s="10" t="n">
         <v>2</v>
@@ -868,7 +876,7 @@
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E18" s="10" t="n">
         <v>2</v>
@@ -882,7 +890,7 @@
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E19" s="10" t="n">
         <v>0</v>
@@ -896,7 +904,7 @@
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E20" s="10" t="n">
         <v>2</v>
@@ -910,79 +918,76 @@
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E21" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>36</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F21" s="10"/>
       <c r="G21" s="9"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="19"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="22" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="F22" s="10"/>
+      <c r="D22" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" s="15"/>
       <c r="G22" s="9"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="15" t="n">
+      <c r="H22" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="5" t="n">
+        <f aca="false">SUM(E24:E27)</f>
+        <v>8</v>
+      </c>
+      <c r="C24" s="5" t="n">
+        <f aca="false">SUM(F24:F27)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="5" t="n">
-        <f aca="false">SUM(E25:E28)</f>
-        <v>8</v>
-      </c>
-      <c r="C25" s="5" t="n">
-        <f aca="false">SUM(F25:F28)</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="7" t="n">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="10"/>
       <c r="G25" s="9"/>
       <c r="H25" s="11"/>
     </row>
@@ -991,7 +996,7 @@
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E26" s="10" t="n">
         <v>2</v>
@@ -1005,7 +1010,7 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E27" s="10" t="n">
         <v>2</v>
@@ -1015,252 +1020,238 @@
       <c r="H27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="11"/>
+      <c r="A28" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
+      <c r="A29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="5" t="n">
+        <f aca="false">SUM(E29:E30)</f>
+        <v>15</v>
+      </c>
+      <c r="C29" s="5" t="n">
+        <f aca="false">SUM(F29:F30)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="5" t="n">
-        <f aca="false">SUM(E30:E31)</f>
-        <v>15</v>
-      </c>
-      <c r="C30" s="5" t="n">
-        <f aca="false">SUM(F30:F31)</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="7" t="n">
-        <v>14</v>
-      </c>
-      <c r="F30" s="7"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="15"/>
       <c r="G30" s="9"/>
       <c r="H30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F31" s="15"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="11"/>
+      <c r="A31" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
+      <c r="A32" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="5" t="n">
+        <f aca="false">SUM(E32:E33)</f>
+        <v>3</v>
+      </c>
+      <c r="C32" s="5" t="n">
+        <f aca="false">SUM(F32:F33)</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="11"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="5" t="n">
-        <f aca="false">SUM(E33:E34)</f>
-        <v>3</v>
-      </c>
-      <c r="C33" s="5" t="n">
-        <f aca="false">SUM(F33:F34)</f>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="F33" s="7"/>
+      <c r="F33" s="15"/>
       <c r="G33" s="9"/>
       <c r="H33" s="11"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="15" t="n">
+      <c r="A34" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="5" t="n">
+        <f aca="false">SUM(E35:E36)</f>
+        <v>5</v>
+      </c>
+      <c r="C35" s="5" t="n">
+        <f aca="false">SUM(F35:F36)</f>
         <v>0</v>
       </c>
-      <c r="F34" s="15"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="11"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
+      <c r="D35" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="11"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="5" t="n">
-        <f aca="false">SUM(E36:E37)</f>
-        <v>5</v>
-      </c>
-      <c r="C36" s="5" t="n">
-        <f aca="false">SUM(F36:F37)</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E36" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="F36" s="7"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="F36" s="15"/>
       <c r="G36" s="9"/>
       <c r="H36" s="11"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E37" s="15" t="n">
+      <c r="A37" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="20" t="n">
+        <f aca="false">E38</f>
+        <v>10</v>
+      </c>
+      <c r="C38" s="20" t="n">
+        <f aca="false">SUM(F38)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="F38" s="22"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="23"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="20" t="n">
+        <f aca="false">E40</f>
         <v>3</v>
       </c>
-      <c r="F37" s="15"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="11"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="21" t="n">
-        <f aca="false">E39</f>
-        <v>10</v>
-      </c>
-      <c r="C39" s="21" t="n">
-        <f aca="false">SUM(F39)</f>
+      <c r="C40" s="20" t="n">
+        <f aca="false">SUM(F40)</f>
         <v>0</v>
       </c>
-      <c r="D39" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="E39" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="F39" s="23"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="24"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="F40" s="22"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="11"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" s="21" t="n">
-        <f aca="false">E41</f>
-        <v>3</v>
-      </c>
-      <c r="C41" s="21" t="n">
-        <f aca="false">SUM(F41)</f>
-        <v>0</v>
-      </c>
-      <c r="D41" s="25"/>
-      <c r="E41" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="F41" s="23"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="11"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B42" s="26" t="n">
-        <f aca="false">SUM(B2:B41)</f>
+      <c r="A41" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="25" t="n">
+        <f aca="false">SUM(B2:B40)</f>
         <v>70</v>
       </c>
-      <c r="C42" s="26" t="n">
-        <f aca="false">SUM(C2:C41)</f>
-        <v>2.25</v>
-      </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="28" t="n">
-        <f aca="false">SUM(E2:E41)</f>
+      <c r="C41" s="25" t="n">
+        <f aca="false">SUM(C2:C40)</f>
+        <v>11</v>
+      </c>
+      <c r="D41" s="26"/>
+      <c r="E41" s="27" t="n">
+        <f aca="false">SUM(E2:E40)</f>
         <v>70</v>
       </c>
-      <c r="F42" s="28" t="n">
-        <f aca="false">SUM(F2:F41)</f>
-        <v>2.25</v>
-      </c>
-      <c r="G42" s="20"/>
-      <c r="H42" s="29"/>
+      <c r="F41" s="27" t="n">
+        <f aca="false">SUM(F2:F40)</f>
+        <v>11</v>
+      </c>
+      <c r="G41" s="19"/>
+      <c r="H41" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -1268,27 +1259,27 @@
     <mergeCell ref="B2:B12"/>
     <mergeCell ref="C2:C12"/>
     <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A14:A23"/>
-    <mergeCell ref="B14:B23"/>
-    <mergeCell ref="C14:C23"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A14:A22"/>
+    <mergeCell ref="B14:B22"/>
+    <mergeCell ref="C14:C22"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A39:H39"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
implements screens & Abnahme
</commit_message>
<xml_diff>
--- a/1. Analyse/Arbeitspakete.xlsx
+++ b/1. Analyse/Arbeitspakete.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
   <si>
     <t>Phasen</t>
   </si>
@@ -194,9 +194,6 @@
   </si>
   <si>
     <t>Implementierung</t>
-  </si>
-  <si>
-    <t>need admin</t>
   </si>
   <si>
     <t>5. Test</t>
@@ -624,22 +621,22 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G39" activeCellId="0" sqref="G39"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="45.4897959183674"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="45.4897959183674"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -971,7 +968,7 @@
       </c>
       <c r="C17" s="5" t="n">
         <f aca="false">SUM(F17:F25)</f>
-        <v>10.25</v>
+        <v>10.75</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>35</v>
@@ -1040,7 +1037,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="10" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>43</v>
@@ -1148,7 +1145,7 @@
       </c>
       <c r="F26" s="19" t="n">
         <f aca="false">SUM(F17:F25)</f>
-        <v>10.25</v>
+        <v>10.75</v>
       </c>
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
@@ -1283,7 +1280,7 @@
       </c>
       <c r="C34" s="5" t="n">
         <f aca="false">SUM(F34:F35)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>56</v>
@@ -1309,10 +1306,10 @@
       <c r="E35" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F35" s="26"/>
-      <c r="G35" s="9" t="s">
-        <v>58</v>
-      </c>
+      <c r="F35" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="G35" s="9"/>
       <c r="H35" s="11"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1326,7 +1323,7 @@
       </c>
       <c r="F36" s="19" t="n">
         <f aca="false">SUM(F34:F35)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G36" s="18"/>
       <c r="H36" s="22"/>
@@ -1345,7 +1342,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" s="5" t="n">
         <f aca="false">SUM(E38:E39)</f>
@@ -1353,15 +1350,17 @@
       </c>
       <c r="C38" s="5" t="n">
         <f aca="false">SUM(F38:F39)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E38" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="F38" s="7"/>
+      <c r="F38" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="G38" s="9"/>
       <c r="H38" s="11"/>
     </row>
@@ -1370,12 +1369,14 @@
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E39" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="F39" s="26"/>
+      <c r="F39" s="26" t="n">
+        <v>0</v>
+      </c>
       <c r="G39" s="9" t="s">
         <v>36</v>
       </c>
@@ -1392,7 +1393,7 @@
       </c>
       <c r="F40" s="19" t="n">
         <f aca="false">SUM(F38:F39)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="18"/>
       <c r="H40" s="22"/>
@@ -1411,7 +1412,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42" s="5" t="n">
         <f aca="false">SUM(E42:E43)</f>
@@ -1419,15 +1420,17 @@
       </c>
       <c r="C42" s="5" t="n">
         <f aca="false">SUM(F42:F43)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E42" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="F42" s="7"/>
+      <c r="F42" s="7" t="n">
+        <v>2</v>
+      </c>
       <c r="G42" s="9"/>
       <c r="H42" s="11"/>
     </row>
@@ -1436,12 +1439,14 @@
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E43" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="F43" s="26"/>
+      <c r="F43" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="G43" s="9"/>
       <c r="H43" s="11"/>
     </row>
@@ -1456,7 +1461,7 @@
       </c>
       <c r="F44" s="19" t="n">
         <f aca="false">SUM(F42:F43)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G44" s="18"/>
       <c r="H44" s="22"/>
@@ -1475,7 +1480,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B46" s="28" t="n">
         <f aca="false">E46</f>
@@ -1483,15 +1488,17 @@
       </c>
       <c r="C46" s="28" t="n">
         <f aca="false">SUM(F46)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E46" s="30" t="n">
         <v>10</v>
       </c>
-      <c r="F46" s="30"/>
+      <c r="F46" s="30" t="n">
+        <v>10</v>
+      </c>
       <c r="G46" s="9"/>
       <c r="H46" s="31"/>
     </row>
@@ -1506,7 +1513,7 @@
       </c>
       <c r="F47" s="19" t="n">
         <f aca="false">SUM(F46)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G47" s="34"/>
       <c r="H47" s="35"/>
@@ -1525,7 +1532,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B49" s="28" t="n">
         <f aca="false">E49</f>
@@ -1545,7 +1552,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B50" s="36" t="n">
         <f aca="false">SUM(B2:B49)</f>
@@ -1553,7 +1560,7 @@
       </c>
       <c r="C50" s="36" t="n">
         <f aca="false">SUM(C2:C49)</f>
-        <v>46.5</v>
+        <v>65</v>
       </c>
       <c r="D50" s="37"/>
       <c r="E50" s="38" t="n">
@@ -1562,7 +1569,7 @@
       </c>
       <c r="F50" s="38" t="n">
         <f aca="false">SUM(F15+F26+F32+F36+F40+F44+F47+F49)</f>
-        <v>46.5</v>
+        <v>65</v>
       </c>
       <c r="G50" s="25"/>
       <c r="H50" s="39"/>

</xml_diff>